<commit_message>
updated the text equations for the logit forest floor consumption model
</commit_message>
<xml_diff>
--- a/GMD/CarbonCalculator.xlsx
+++ b/GMD/CarbonCalculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danthomp\Documents\nrcan-cfs-fire\FireDMs\GMD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0E233A4-6C4C-4803-8AE7-08AFCF9DD249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC02CC3F-F92E-4CCE-9EE1-2DACC31DE6D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="48" windowWidth="30936" windowHeight="17040" xr2:uid="{16CE1E83-2308-4ECC-BD41-9B5C697359CE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17040" xr2:uid="{16CE1E83-2308-4ECC-BD41-9B5C697359CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -116,7 +116,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -157,7 +157,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,7 +475,7 @@
   <dimension ref="A1:W20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z5" sqref="I3:Z5"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -518,8 +518,8 @@
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <f>T9</f>
-        <v>0.8801783753501401</v>
+        <f t="shared" ref="B2:B8" si="0">T9</f>
+        <v>0.8677203921568627</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -534,14 +534,14 @@
         <v>4</v>
       </c>
       <c r="B3" s="2">
-        <f>T10</f>
+        <f t="shared" si="0"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D15" si="0">_xlfn.CONCAT(C3,A3)</f>
+        <f t="shared" ref="D3:D15" si="1">_xlfn.CONCAT(C3,A3)</f>
         <v>FlamingCO</v>
       </c>
     </row>
@@ -550,14 +550,14 @@
         <v>9</v>
       </c>
       <c r="B4" s="2">
-        <f>T11</f>
-        <v>1.6E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
       </c>
       <c r="D4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>FlamingPM10</v>
       </c>
     </row>
@@ -566,14 +566,14 @@
         <v>6</v>
       </c>
       <c r="B5" s="2">
-        <f>T12</f>
+        <f t="shared" si="0"/>
         <v>1.6E-2</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
       </c>
       <c r="D5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>FlamingNMOG</v>
       </c>
       <c r="Q5" t="s">
@@ -588,14 +588,14 @@
         <v>23</v>
       </c>
       <c r="B6" s="2">
-        <f>T13</f>
-        <v>1.2999999999999999E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.9E-2</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
       </c>
       <c r="D6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>FlamingPM25</v>
       </c>
       <c r="I6" t="s">
@@ -628,14 +628,14 @@
         <v>3</v>
       </c>
       <c r="B7" s="2">
-        <f>T14</f>
+        <f t="shared" si="0"/>
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="C7" t="s">
         <v>0</v>
       </c>
       <c r="D7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>FlamingCH4</v>
       </c>
       <c r="I7" t="s">
@@ -647,14 +647,14 @@
         <v>5</v>
       </c>
       <c r="B8" s="2">
-        <f>T15</f>
+        <f t="shared" si="0"/>
         <v>1E-3</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
       </c>
       <c r="D8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>FlamingBC</v>
       </c>
       <c r="I8" t="s">
@@ -666,14 +666,14 @@
         <v>2</v>
       </c>
       <c r="B9" s="2">
-        <f>U9</f>
-        <v>0.72918445378151264</v>
+        <f t="shared" ref="B9:B15" si="2">U9</f>
+        <v>0.70274327731092445</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
       </c>
       <c r="D9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>SmoulderingCO2</v>
       </c>
       <c r="I9" t="s">
@@ -681,19 +681,19 @@
       </c>
       <c r="Q9" s="3">
         <f>$K$1-SUM(Q10:Q18)</f>
-        <v>448.89097142857145</v>
+        <v>442.53739999999999</v>
       </c>
       <c r="R9" s="3">
         <f>$K$1-SUM(R10:R18)</f>
-        <v>371.88407142857147</v>
+        <v>358.39907142857146</v>
       </c>
       <c r="T9" s="2">
         <f>Q9/$K$1</f>
-        <v>0.8801783753501401</v>
+        <v>0.8677203921568627</v>
       </c>
       <c r="U9" s="2">
         <f>R9/$K$1</f>
-        <v>0.72918445378151264</v>
+        <v>0.70274327731092445</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
@@ -701,14 +701,14 @@
         <v>4</v>
       </c>
       <c r="B10" s="2">
-        <f>U10</f>
+        <f t="shared" si="2"/>
         <v>0.161</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
       </c>
       <c r="D10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>SmoulderingCO</v>
       </c>
       <c r="I10" t="s">
@@ -732,19 +732,19 @@
         <v>191.5</v>
       </c>
       <c r="Q10" s="3">
-        <f>K10*J10</f>
+        <f t="shared" ref="Q10:Q15" si="3">K10*J10</f>
         <v>35.571428571428569</v>
       </c>
       <c r="R10" s="3">
-        <f>N10*J10</f>
+        <f t="shared" ref="R10:R15" si="4">N10*J10</f>
         <v>82.071428571428569</v>
       </c>
       <c r="T10" s="2">
-        <f>ROUND(Q10/$K$1,3)</f>
+        <f t="shared" ref="T10:U15" si="5">ROUND(Q10/$K$1,3)</f>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="U10" s="2">
-        <f>ROUND(R10/$K$1,3)</f>
+        <f t="shared" si="5"/>
         <v>0.161</v>
       </c>
     </row>
@@ -753,21 +753,22 @@
         <v>9</v>
       </c>
       <c r="B11" s="2">
-        <f>U11</f>
-        <v>3.3000000000000002E-2</v>
+        <f t="shared" si="2"/>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>
       </c>
       <c r="D11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>SmoulderingPM10</v>
       </c>
       <c r="I11" t="s">
         <v>9</v>
       </c>
       <c r="J11" s="1">
-        <v>0.5</v>
+        <f>1/1.4</f>
+        <v>0.7142857142857143</v>
       </c>
       <c r="K11">
         <v>16.05</v>
@@ -784,19 +785,19 @@
       </c>
       <c r="Q11" s="3">
         <f>K11*J11</f>
-        <v>8.0250000000000004</v>
+        <v>11.464285714285715</v>
       </c>
       <c r="R11" s="3">
         <f>N11*J11</f>
-        <v>17.032499999999999</v>
+        <v>24.332142857142856</v>
       </c>
       <c r="T11" s="2">
-        <f>ROUND(Q11/$K$1,3)</f>
-        <v>1.6E-2</v>
+        <f t="shared" si="5"/>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="U11" s="2">
-        <f>ROUND(R11/$K$1,3)</f>
-        <v>3.3000000000000002E-2</v>
+        <f t="shared" si="5"/>
+        <v>4.8000000000000001E-2</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
@@ -804,14 +805,14 @@
         <v>6</v>
       </c>
       <c r="B12" s="2">
-        <f>U12</f>
+        <f t="shared" si="2"/>
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="C12" t="s">
         <v>1</v>
       </c>
       <c r="D12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>SmoulderingNMOG</v>
       </c>
       <c r="I12" t="s">
@@ -835,19 +836,19 @@
         <v>44.974999999999994</v>
       </c>
       <c r="Q12" s="3">
-        <f>K12*J12</f>
+        <f t="shared" si="3"/>
         <v>7.9400000000000013</v>
       </c>
       <c r="R12" s="3">
-        <f>N12*J12</f>
+        <f t="shared" si="4"/>
         <v>17.989999999999998</v>
       </c>
       <c r="T12" s="2">
-        <f>ROUND(Q12/$K$1,3)</f>
+        <f t="shared" si="5"/>
         <v>1.6E-2</v>
       </c>
       <c r="U12" s="2">
-        <f>ROUND(R12/$K$1,3)</f>
+        <f t="shared" si="5"/>
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="W12" t="s">
@@ -859,21 +860,22 @@
         <v>23</v>
       </c>
       <c r="B13" s="2">
-        <f>U13</f>
-        <v>2.8000000000000001E-2</v>
+        <f t="shared" si="2"/>
+        <v>0.04</v>
       </c>
       <c r="C13" t="s">
         <v>1</v>
       </c>
       <c r="D13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>SmoulderingPM25</v>
       </c>
       <c r="I13" t="s">
         <v>10</v>
       </c>
       <c r="J13" s="1">
-        <v>0.5</v>
+        <f>1/1.4</f>
+        <v>0.7142857142857143</v>
       </c>
       <c r="K13">
         <v>13.6</v>
@@ -889,20 +891,20 @@
         <v>28.865000000000002</v>
       </c>
       <c r="Q13" s="3">
-        <f>K13*J13</f>
-        <v>6.8</v>
+        <f t="shared" si="3"/>
+        <v>9.7142857142857135</v>
       </c>
       <c r="R13" s="3">
-        <f>N13*J13</f>
-        <v>14.432500000000001</v>
+        <f t="shared" si="4"/>
+        <v>20.617857142857144</v>
       </c>
       <c r="T13" s="2">
-        <f>ROUND(Q13/$K$1,3)</f>
-        <v>1.2999999999999999E-2</v>
+        <f t="shared" si="5"/>
+        <v>1.9E-2</v>
       </c>
       <c r="U13" s="2">
-        <f>ROUND(R13/$K$1,3)</f>
-        <v>2.8000000000000001E-2</v>
+        <f t="shared" si="5"/>
+        <v>0.04</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.3">
@@ -910,14 +912,14 @@
         <v>3</v>
       </c>
       <c r="B14" s="2">
-        <f>U14</f>
+        <f t="shared" si="2"/>
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="C14" t="s">
         <v>1</v>
       </c>
       <c r="D14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>SmoulderingCH4</v>
       </c>
       <c r="I14" t="s">
@@ -941,19 +943,19 @@
         <v>8.629999999999999</v>
       </c>
       <c r="Q14" s="3">
-        <f>K14*J14</f>
+        <f t="shared" si="3"/>
         <v>2.4224999999999999</v>
       </c>
       <c r="R14" s="3">
-        <f>N14*J14</f>
+        <f t="shared" si="4"/>
         <v>6.4724999999999993</v>
       </c>
       <c r="T14" s="2">
-        <f>ROUND(Q14/$K$1,3)</f>
+        <f t="shared" si="5"/>
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="U14" s="2">
-        <f>ROUND(R14/$K$1,3)</f>
+        <f t="shared" si="5"/>
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
@@ -962,14 +964,14 @@
         <v>5</v>
       </c>
       <c r="B15" s="2">
-        <f>U15</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C15" t="s">
         <v>1</v>
       </c>
       <c r="D15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>SmoulderingBC</v>
       </c>
       <c r="I15" t="s">
@@ -985,19 +987,19 @@
         <v>0.13</v>
       </c>
       <c r="Q15" s="3">
-        <f>K15*J15</f>
+        <f t="shared" si="3"/>
         <v>0.35010000000000002</v>
       </c>
       <c r="R15" s="3">
-        <f>N15*J15</f>
+        <f t="shared" si="4"/>
         <v>0.11700000000000001</v>
       </c>
       <c r="T15" s="2">
-        <f>ROUND(Q15/$K$1,3)</f>
+        <f t="shared" si="5"/>
         <v>1E-3</v>
       </c>
       <c r="U15" s="2">
-        <f>ROUND(R15/$K$1,3)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -1025,11 +1027,11 @@
       </c>
       <c r="Q20">
         <f>Q9/(12/(12+16+16))</f>
-        <v>1645.9335619047622</v>
+        <v>1622.6371333333334</v>
       </c>
       <c r="R20">
         <f>R9/(12/(12+16+16))</f>
-        <v>1363.5749285714289</v>
+        <v>1314.1299285714288</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Got first draft of PM2.5 pools working as a big loop
</commit_message>
<xml_diff>
--- a/GMD/CarbonCalculator.xlsx
+++ b/GMD/CarbonCalculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danthomp\Documents\nrcan-cfs-fire\FireDMs\GMD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC02CC3F-F92E-4CCE-9EE1-2DACC31DE6D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D753419-688C-4AD7-B9D6-C1B519626FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17040" xr2:uid="{16CE1E83-2308-4ECC-BD41-9B5C697359CE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{16CE1E83-2308-4ECC-BD41-9B5C697359CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="34">
   <si>
     <t>Flaming</t>
   </si>
@@ -108,6 +108,36 @@
   </si>
   <si>
     <t>PM25</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>Frac Consunm</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>InvLogit(FracConsump)</t>
+  </si>
+  <si>
+    <t>Duff Load (kg m2)</t>
+  </si>
+  <si>
+    <t>PM2.5:CO</t>
+  </si>
+  <si>
+    <t>PM10:CO</t>
+  </si>
+  <si>
+    <t>NMOG:CO</t>
   </si>
 </sst>
 </file>
@@ -472,22 +502,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{833BF93D-B5EB-44A4-8D79-99DFA59B7D70}">
-  <dimension ref="A1:W20"/>
+  <dimension ref="A1:W29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="U22" sqref="U22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="32" customWidth="1"/>
-    <col min="4" max="4" width="16.88671875" customWidth="1"/>
-    <col min="5" max="6" width="11.33203125" customWidth="1"/>
-    <col min="11" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.109375" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" customWidth="1"/>
+    <col min="19" max="19" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -513,7 +545,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -529,7 +561,7 @@
         <v>FlamingCO2</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -545,7 +577,7 @@
         <v>FlamingCO</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -561,7 +593,7 @@
         <v>FlamingPM10</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -583,7 +615,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -622,8 +654,14 @@
       <c r="R6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="T6" t="s">
+        <v>0</v>
+      </c>
+      <c r="U6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -642,7 +680,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -661,7 +699,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -696,7 +734,7 @@
         <v>0.70274327731092445</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -748,7 +786,7 @@
         <v>0.161</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -800,7 +838,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -855,7 +893,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -907,7 +945,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -959,7 +997,7 @@
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -1003,25 +1041,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
       <c r="T16" s="2"/>
       <c r="U16" s="2"/>
     </row>
-    <row r="17" spans="16:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:21" x14ac:dyDescent="0.25">
       <c r="Q17" s="3"/>
       <c r="R17" s="3"/>
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
     </row>
-    <row r="18" spans="16:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:21" x14ac:dyDescent="0.25">
       <c r="Q18" s="3"/>
       <c r="R18" s="3"/>
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
     </row>
-    <row r="20" spans="16:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:21" x14ac:dyDescent="0.25">
       <c r="P20" t="s">
         <v>17</v>
       </c>
@@ -1032,6 +1070,132 @@
       <c r="R20">
         <f>R9/(12/(12+16+16))</f>
         <v>1314.1299285714288</v>
+      </c>
+      <c r="S20" t="s">
+        <v>31</v>
+      </c>
+      <c r="T20">
+        <f>T13/T$10</f>
+        <v>0.27142857142857141</v>
+      </c>
+      <c r="U20">
+        <f>U13/U$10</f>
+        <v>0.2484472049689441</v>
+      </c>
+    </row>
+    <row r="21" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="S21" t="s">
+        <v>32</v>
+      </c>
+      <c r="T21">
+        <f>T11/T$10</f>
+        <v>0.31428571428571422</v>
+      </c>
+      <c r="U21">
+        <f>U11/U$10</f>
+        <v>0.29813664596273293</v>
+      </c>
+    </row>
+    <row r="22" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="S22" t="s">
+        <v>33</v>
+      </c>
+      <c r="T22">
+        <f>T12/T$10</f>
+        <v>0.22857142857142856</v>
+      </c>
+      <c r="U22">
+        <f>U12/U$10</f>
+        <v>0.21739130434782611</v>
+      </c>
+    </row>
+    <row r="23" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>0.33</v>
+      </c>
+      <c r="D24">
+        <v>-0.17</v>
+      </c>
+      <c r="E24">
+        <v>-4.8</v>
+      </c>
+    </row>
+    <row r="25" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" t="s">
+        <v>30</v>
+      </c>
+      <c r="E25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>200</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <f t="shared" ref="E26:E28" si="6">(C26^$C$24)*(D26^$D$24)+$E$24</f>
+        <v>0.94565967681867313</v>
+      </c>
+      <c r="F26">
+        <f>EXP(E26)/(1+EXP(E26))</f>
+        <v>0.72024146683083701</v>
+      </c>
+    </row>
+    <row r="27" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>200</v>
+      </c>
+      <c r="D27">
+        <v>3</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="6"/>
+        <v>-3.3174155995569166E-2</v>
+      </c>
+      <c r="F27">
+        <f t="shared" ref="F27:F28" si="7">EXP(E27)/(1+EXP(E27))</f>
+        <v>0.49170722152106949</v>
+      </c>
+    </row>
+    <row r="28" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>200</v>
+      </c>
+      <c r="D28">
+        <v>5</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="6"/>
+        <v>-0.42966228759965119</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="7"/>
+        <v>0.39420697705381963</v>
+      </c>
+    </row>
+    <row r="29" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>